<commit_message>
other simiarity done, but result not good
</commit_message>
<xml_diff>
--- a/Vincent/Excel_analyze/Exp7(MGM fitting)/PosSimScaling res/SimPosAna.xlsx
+++ b/Vincent/Excel_analyze/Exp7(MGM fitting)/PosSimScaling res/SimPosAna.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4155" windowHeight="3285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4155" windowHeight="3285" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PosGeneral_SimGau" sheetId="1" r:id="rId1"/>
     <sheet name="PosGeneral_SimCorrcoef" sheetId="2" r:id="rId2"/>
     <sheet name="Possibility" sheetId="3" r:id="rId3"/>
+    <sheet name="PosGen_SimFrechet" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="73">
   <si>
     <t>Original Matching</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1139,11 +1140,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="368291336"/>
-        <c:axId val="368286632"/>
+        <c:axId val="359375520"/>
+        <c:axId val="359377088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="368291336"/>
+        <c:axId val="359375520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1200,12 +1201,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368286632"/>
+        <c:crossAx val="359377088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="368286632"/>
+        <c:axId val="359377088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1262,7 +1263,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368291336"/>
+        <c:crossAx val="359375520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1507,11 +1508,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="430520512"/>
-        <c:axId val="430518160"/>
+        <c:axId val="360497568"/>
+        <c:axId val="360498744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="430520512"/>
+        <c:axId val="360497568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1568,12 +1569,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430518160"/>
+        <c:crossAx val="360498744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="430518160"/>
+        <c:axId val="360498744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1630,7 +1631,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430520512"/>
+        <c:crossAx val="360497568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1875,11 +1876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="430517768"/>
-        <c:axId val="430524824"/>
+        <c:axId val="360502664"/>
+        <c:axId val="360504232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="430517768"/>
+        <c:axId val="360502664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1936,12 +1937,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430524824"/>
+        <c:crossAx val="360504232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="430524824"/>
+        <c:axId val="360504232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1998,7 +1999,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430517768"/>
+        <c:crossAx val="360502664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2268,11 +2269,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="434576360"/>
-        <c:axId val="434568520"/>
+        <c:axId val="359378656"/>
+        <c:axId val="359379048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="434576360"/>
+        <c:axId val="359378656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2329,12 +2330,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="434568520"/>
+        <c:crossAx val="359379048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="434568520"/>
+        <c:axId val="359379048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2391,7 +2392,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="434576360"/>
+        <c:crossAx val="359378656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2624,11 +2625,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="434567736"/>
-        <c:axId val="434573616"/>
+        <c:axId val="359371992"/>
+        <c:axId val="359372384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="434567736"/>
+        <c:axId val="359371992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2685,12 +2686,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="434573616"/>
+        <c:crossAx val="359372384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="434573616"/>
+        <c:axId val="359372384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2747,7 +2748,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="434567736"/>
+        <c:crossAx val="359371992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3025,11 +3026,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="434581064"/>
-        <c:axId val="434569304"/>
+        <c:axId val="427146480"/>
+        <c:axId val="427144912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="434581064"/>
+        <c:axId val="427146480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3086,12 +3087,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="434569304"/>
+        <c:crossAx val="427144912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="434569304"/>
+        <c:axId val="427144912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3148,7 +3149,1141 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="434581064"/>
+        <c:crossAx val="427146480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Band1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PosGen_SimFrechet!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Amount</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="zh-CN"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PosGen_SimFrechet!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.3730000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1232000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6077E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6794E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1180999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.9152999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PosGen_SimFrechet!$J$3:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.8330000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6160000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.175</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8660000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3759999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="427140992"/>
+        <c:axId val="430157312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="427140992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="430157312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="430157312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="427140992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Band2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PosGen_SimFrechet!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Amount</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PosGen_SimFrechet!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.106961</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14255999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.101796</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17202100000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.128048</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.12737899999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PosGen_SimFrechet!$J$3:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.8330000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6160000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.175</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8660000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3759999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="506495448"/>
+        <c:axId val="506494664"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="506495448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="506494664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="506494664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="506495448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Band3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PosGen_SimFrechet!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Amount</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="zh-CN"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PosGen_SimFrechet!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.8923000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0711E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6929E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0801E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.162E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.7139999999999995E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PosGen_SimFrechet!$J$3:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.8330000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6160000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.175</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8660000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3759999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="506494272"/>
+        <c:axId val="506492312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="506494272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="506492312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="506492312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="506494272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3393,11 +4528,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="368292512"/>
-        <c:axId val="368293688"/>
+        <c:axId val="359375912"/>
+        <c:axId val="359375128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="368292512"/>
+        <c:axId val="359375912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3454,12 +4589,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368293688"/>
+        <c:crossAx val="359375128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="368293688"/>
+        <c:axId val="359375128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3516,7 +4651,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368292512"/>
+        <c:crossAx val="359375912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3761,11 +4896,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="368292904"/>
-        <c:axId val="368287808"/>
+        <c:axId val="359374736"/>
+        <c:axId val="359378264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="368292904"/>
+        <c:axId val="359374736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3822,12 +4957,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368287808"/>
+        <c:crossAx val="359378264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="368287808"/>
+        <c:axId val="359378264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3884,7 +5019,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368292904"/>
+        <c:crossAx val="359374736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4129,11 +5264,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="368287416"/>
-        <c:axId val="368289768"/>
+        <c:axId val="359372776"/>
+        <c:axId val="359373168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="368287416"/>
+        <c:axId val="359372776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4190,12 +5325,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368289768"/>
+        <c:crossAx val="359373168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="368289768"/>
+        <c:axId val="359373168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4252,7 +5387,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368287416"/>
+        <c:crossAx val="359372776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4451,11 +5586,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="368293296"/>
-        <c:axId val="368294080"/>
+        <c:axId val="359374344"/>
+        <c:axId val="360499136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="368293296"/>
+        <c:axId val="359374344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4512,12 +5647,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368294080"/>
+        <c:crossAx val="360499136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="368294080"/>
+        <c:axId val="360499136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4574,7 +5709,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368293296"/>
+        <c:crossAx val="359374344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4817,11 +5952,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="368290160"/>
-        <c:axId val="368290552"/>
+        <c:axId val="360503056"/>
+        <c:axId val="360499528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="368290160"/>
+        <c:axId val="360503056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4878,12 +6013,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368290552"/>
+        <c:crossAx val="360499528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="368290552"/>
+        <c:axId val="360499528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4940,7 +6075,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368290160"/>
+        <c:crossAx val="360503056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5185,11 +6320,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="368288200"/>
-        <c:axId val="368292120"/>
+        <c:axId val="360497176"/>
+        <c:axId val="360501880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="368288200"/>
+        <c:axId val="360497176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5246,12 +6381,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368292120"/>
+        <c:crossAx val="360501880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="368292120"/>
+        <c:axId val="360501880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5308,7 +6443,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="368288200"/>
+        <c:crossAx val="360497176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5553,11 +6688,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="430522080"/>
-        <c:axId val="430520120"/>
+        <c:axId val="360501488"/>
+        <c:axId val="360500312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="430522080"/>
+        <c:axId val="360501488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5614,12 +6749,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430520120"/>
+        <c:crossAx val="360500312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="430520120"/>
+        <c:axId val="360500312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5676,7 +6811,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430522080"/>
+        <c:crossAx val="360501488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5921,11 +7056,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="430519336"/>
-        <c:axId val="430521296"/>
+        <c:axId val="360501096"/>
+        <c:axId val="360503448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="430519336"/>
+        <c:axId val="360501096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5982,12 +7117,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430521296"/>
+        <c:crossAx val="360503448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="430521296"/>
+        <c:axId val="360503448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6044,7 +7179,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430519336"/>
+        <c:crossAx val="360501096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6294,6 +7429,126 @@
 </file>
 
 <file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -9234,6 +10489,1554 @@
 </file>
 
 <file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -14312,6 +17115,101 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1243012</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>147637</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>52387</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>176212</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1166812</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>71437</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -14577,8 +17475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -15969,7 +18867,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J8" sqref="A1:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -16239,4 +19137,278 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="13.875" customWidth="1"/>
+    <col min="3" max="3" width="11.75" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="13.875" customWidth="1"/>
+    <col min="6" max="6" width="13.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A2" s="5"/>
+      <c r="B2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="5">
+        <v>7.3730000000000004E-2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.106961</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2.8923000000000001E-2</v>
+      </c>
+      <c r="E3" s="5">
+        <f>AVERAGE(B3:D3)</f>
+        <v>6.9871333333333327E-2</v>
+      </c>
+      <c r="F3" s="5">
+        <f>0.5*B3+0.3*C3+0.2*D3</f>
+        <v>7.4737899999999996E-2</v>
+      </c>
+      <c r="G3" s="12">
+        <v>9.7620000000000005</v>
+      </c>
+      <c r="H3" s="14">
+        <v>9.8360000000000003</v>
+      </c>
+      <c r="I3" s="16">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J3" s="6">
+        <v>2.8330000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="5">
+        <v>6.1232000000000002E-2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.14255999999999999</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2.0711E-2</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" ref="E4:E8" si="0">AVERAGE(B4:D4)</f>
+        <v>7.4834333333333336E-2</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" ref="F4:F8" si="1">0.5*B4+0.3*C4+0.2*D4</f>
+        <v>7.752619999999999E-2</v>
+      </c>
+      <c r="G4" s="13">
+        <v>8.6479999999999997</v>
+      </c>
+      <c r="H4" s="15">
+        <v>10.317</v>
+      </c>
+      <c r="I4" s="17">
+        <v>1.2170000000000001</v>
+      </c>
+      <c r="J4" s="7">
+        <v>2.4220000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="5">
+        <v>4.6077E-2</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.101796</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1.6929E-2</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
+        <v>5.4934000000000004E-2</v>
+      </c>
+      <c r="F5" s="5">
+        <f t="shared" si="1"/>
+        <v>5.6963099999999996E-2</v>
+      </c>
+      <c r="G5" s="13">
+        <v>5.516</v>
+      </c>
+      <c r="H5" s="15">
+        <v>9.2829999999999995</v>
+      </c>
+      <c r="I5" s="17">
+        <v>1.0509999999999999</v>
+      </c>
+      <c r="J5" s="7">
+        <v>1.6160000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="5">
+        <v>3.6794E-2</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.17202100000000001</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1.0801E-2</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
+        <v>7.3205333333333331E-2</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" si="1"/>
+        <v>7.2163500000000005E-2</v>
+      </c>
+      <c r="G6" s="13">
+        <v>4.2450000000000001</v>
+      </c>
+      <c r="H6" s="15">
+        <v>6.8460000000000001</v>
+      </c>
+      <c r="I6" s="17">
+        <v>1.1040000000000001</v>
+      </c>
+      <c r="J6" s="7">
+        <v>1.175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="5">
+        <v>5.1180999999999997E-2</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.128048</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2.162E-2</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
+        <v>6.6949666666666671E-2</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="1"/>
+        <v>6.8328899999999984E-2</v>
+      </c>
+      <c r="G7" s="13">
+        <v>6.68</v>
+      </c>
+      <c r="H7" s="15">
+        <v>7.2</v>
+      </c>
+      <c r="I7" s="17">
+        <v>1.006</v>
+      </c>
+      <c r="J7" s="7">
+        <v>1.8660000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2.9152999999999998E-2</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.12737899999999999</v>
+      </c>
+      <c r="D8" s="5">
+        <v>8.7139999999999995E-3</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>5.5081999999999999E-2</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="1"/>
+        <v>5.4532999999999998E-2</v>
+      </c>
+      <c r="G8" s="13">
+        <v>4.5990000000000002</v>
+      </c>
+      <c r="H8" s="15">
+        <v>8.0709999999999997</v>
+      </c>
+      <c r="I8" s="17">
+        <v>1.2490000000000001</v>
+      </c>
+      <c r="J8" s="7">
+        <v>1.3759999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>